<commit_message>
Hazards catalog, hazards, lots of components.
</commit_message>
<xml_diff>
--- a/Stats.xlsx
+++ b/Stats.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Unity Projects\Project-SpaceMage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{063CBD97-5D14-4F18-8A6C-BC506220AB3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC13B31E-16FD-4D2D-8A57-4632C584CB4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{C7E500E0-3096-4EFE-AE2D-B6684D65CA8F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{C7E500E0-3096-4EFE-AE2D-B6684D65CA8F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Ships" sheetId="1" r:id="rId1"/>
-    <sheet name="Engines" sheetId="2" r:id="rId2"/>
-    <sheet name="Magic Spheres" sheetId="3" r:id="rId3"/>
+    <sheet name="Functionality" sheetId="4" r:id="rId1"/>
+    <sheet name="Ships" sheetId="1" r:id="rId2"/>
+    <sheet name="Engines" sheetId="2" r:id="rId3"/>
+    <sheet name="Magic Spheres" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="Engines">Engines!$A$2:$A$12</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
   <si>
     <t>Name</t>
   </si>
@@ -82,13 +83,85 @@
   </si>
   <si>
     <t>Inertia Recovery</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Details</t>
+  </si>
+  <si>
+    <t>Functionality</t>
+  </si>
+  <si>
+    <t>IDieTarget</t>
+  </si>
+  <si>
+    <t>This is just an optional component if Die() needs to kill a parent.</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Idie</t>
+  </si>
+  <si>
+    <t>Destroys the gameObject, or the IDieTarget gameObject if specified.</t>
+  </si>
+  <si>
+    <t>Die()</t>
+  </si>
+  <si>
+    <t>ITakeDamage</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>GameObject that dies</t>
+  </si>
+  <si>
+    <t>Requirements</t>
+  </si>
+  <si>
+    <t>Health</t>
+  </si>
+  <si>
+    <t>Tracks the max and current health of an entity.</t>
+  </si>
+  <si>
+    <t>Max, Current</t>
+  </si>
+  <si>
+    <t>Change(amount +/-)</t>
+  </si>
+  <si>
+    <t>IDealImpactDamage</t>
+  </si>
+  <si>
+    <t>Accepts incoming damage and reduces current health appropriately.</t>
+  </si>
+  <si>
+    <t>TakeDamage(amount +, collisionSpeed = 0)</t>
+  </si>
+  <si>
+    <t>Health, Idie, MinSpeedForImpactDamage, ExtraSpeedDamageMultiplier</t>
+  </si>
+  <si>
+    <t>RigidBody2D, ImpactBaseDamage, DamageInterval</t>
+  </si>
+  <si>
+    <t>OnCollisionEnter2D(dealImpactDamage(ITakeDamage damageableTarget, float collisionSpeed)</t>
+  </si>
+  <si>
+    <t>Attempts to deal damage to anything that collides with it. Can limit frequency.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,6 +176,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -125,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -140,6 +226,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,10 +541,136 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE64B771-968C-46C8-9271-EDE5A665D12D}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.140625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="53.42578125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="51" style="7" customWidth="1"/>
+    <col min="5" max="5" width="85.28515625" style="7" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="6" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+      <c r="A1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CB6BFD2-CE5A-40F4-BA92-3147B81EA9BB}">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
@@ -541,7 +755,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{144A139D-D533-44EB-AD22-9EAD17500748}">
   <dimension ref="A1:Q13"/>
   <sheetViews>
@@ -617,7 +831,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F9F5913-872F-4EF1-9FC5-09C660CB0FB2}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Worked on spawning from death, refactored Actor components, and started work with UIToolkit.
</commit_message>
<xml_diff>
--- a/Stats.xlsx
+++ b/Stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Unity Projects\Project-SpaceMage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC13B31E-16FD-4D2D-8A57-4632C584CB4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11F0ECC6-CC4B-48BA-873C-1CE90FC61FDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{C7E500E0-3096-4EFE-AE2D-B6684D65CA8F}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="85">
   <si>
     <t>Name</t>
   </si>
@@ -91,36 +91,9 @@
     <t>Details</t>
   </si>
   <si>
-    <t>Functionality</t>
-  </si>
-  <si>
-    <t>IDieTarget</t>
-  </si>
-  <si>
-    <t>This is just an optional component if Die() needs to kill a parent.</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
-    <t>Idie</t>
-  </si>
-  <si>
-    <t>Destroys the gameObject, or the IDieTarget gameObject if specified.</t>
-  </si>
-  <si>
-    <t>Die()</t>
-  </si>
-  <si>
-    <t>ITakeDamage</t>
-  </si>
-  <si>
-    <t>Data</t>
-  </si>
-  <si>
-    <t>GameObject that dies</t>
-  </si>
-  <si>
     <t>Requirements</t>
   </si>
   <si>
@@ -133,35 +106,203 @@
     <t>Max, Current</t>
   </si>
   <si>
-    <t>Change(amount +/-)</t>
-  </si>
-  <si>
-    <t>IDealImpactDamage</t>
-  </si>
-  <si>
-    <t>Accepts incoming damage and reduces current health appropriately.</t>
-  </si>
-  <si>
-    <t>TakeDamage(amount +, collisionSpeed = 0)</t>
-  </si>
-  <si>
-    <t>Health, Idie, MinSpeedForImpactDamage, ExtraSpeedDamageMultiplier</t>
-  </si>
-  <si>
-    <t>RigidBody2D, ImpactBaseDamage, DamageInterval</t>
-  </si>
-  <si>
-    <t>OnCollisionEnter2D(dealImpactDamage(ITakeDamage damageableTarget, float collisionSpeed)</t>
-  </si>
-  <si>
-    <t>Attempts to deal damage to anything that collides with it. Can limit frequency.</t>
+    <t>Folder</t>
+  </si>
+  <si>
+    <t>Camera</t>
+  </si>
+  <si>
+    <t>CameraFollows</t>
+  </si>
+  <si>
+    <t>The camera will follow this object elastically.</t>
+  </si>
+  <si>
+    <t>Death</t>
+  </si>
+  <si>
+    <t>DieFromHealthLoss</t>
+  </si>
+  <si>
+    <t>Public Functionality</t>
+  </si>
+  <si>
+    <t>Actor</t>
+  </si>
+  <si>
+    <t>ActorManager</t>
+  </si>
+  <si>
+    <t>ActorPool</t>
+  </si>
+  <si>
+    <t>Tracks ActorPools. Handles Actor Instantiation and activation.</t>
+  </si>
+  <si>
+    <t>Static Instantiates.</t>
+  </si>
+  <si>
+    <t>Contains a list of Actors to avoid instantiation &amp; destruction calls.</t>
+  </si>
+  <si>
+    <t>An entity that can be interacted with in some way. Tracks status in pool.</t>
+  </si>
+  <si>
+    <t>RigidBody2D</t>
+  </si>
+  <si>
+    <t>FilterData, SpawnPool, IsWaitingInPool</t>
+  </si>
+  <si>
+    <t>ActorPools - Primary, Secondary, Tertiary, Quaternary</t>
+  </si>
+  <si>
+    <t>EVENTS</t>
+  </si>
+  <si>
+    <t>ActivateInPoolEvent, WaitInPoolEvent</t>
+  </si>
+  <si>
+    <t>ActivateInPool, WaitInPool (both referenced by ActorManager only)</t>
+  </si>
+  <si>
+    <t>TargetCamera, IsTethered, MaxDistance, FollowSpeed</t>
+  </si>
+  <si>
+    <t>Defense</t>
+  </si>
+  <si>
+    <t>Max, Current, IsFull, Fill, Set, Reduce, Increase</t>
+  </si>
+  <si>
+    <t>DoNotRotate</t>
+  </si>
+  <si>
+    <t>MotionLimiter</t>
+  </si>
+  <si>
+    <t>NoOverlap</t>
+  </si>
+  <si>
+    <t>TorqueRemover</t>
+  </si>
+  <si>
+    <t>SpawnWithMotion</t>
+  </si>
+  <si>
+    <t>Mobility</t>
+  </si>
+  <si>
+    <t>Keep this object from rotating at all times.</t>
+  </si>
+  <si>
+    <t>Dies at a health threshold (actor waits in pool).</t>
+  </si>
+  <si>
+    <t>Health, (Actor)</t>
+  </si>
+  <si>
+    <t>DiesAt</t>
+  </si>
+  <si>
+    <t>Public Data</t>
+  </si>
+  <si>
+    <t>List&lt;Actor&gt; Actors</t>
+  </si>
+  <si>
+    <t>Clamps rigidbody rotation and velocity to a minimum and maximum.</t>
+  </si>
+  <si>
+    <t>VelocityRange, RotationRange</t>
+  </si>
+  <si>
+    <t>SetMaxVelocity, SetMinVelocity, SetMaxRotation, SetMinRotation</t>
+  </si>
+  <si>
+    <t>GetWaitingActorByPrefabId - returns null if none found.</t>
+  </si>
+  <si>
+    <t>Force overlapping colliders, that can collide, to push each other away until they no longer overlap.</t>
+  </si>
+  <si>
+    <t>Impart velocity and/or rotation to this rigidody when it spawns (or activates). The velocity and/or rotation may be influenced by the parent's velocity and rotation.</t>
+  </si>
+  <si>
+    <t>Momentum, AngleRange, VelocityRange, RotationRange</t>
+  </si>
+  <si>
+    <t>ImpartMotion</t>
+  </si>
+  <si>
+    <t>Reduce rigidbody angular velocity to zero over time.</t>
+  </si>
+  <si>
+    <t>Rate</t>
+  </si>
+  <si>
+    <t>DamageOnCollision</t>
+  </si>
+  <si>
+    <t>Offense</t>
+  </si>
+  <si>
+    <t>Damage, IntervalInFrames</t>
+  </si>
+  <si>
+    <t>Deals damage with anything it collides with. Will get rigidbody from parent if it doesn't have one.</t>
+  </si>
+  <si>
+    <t>CollidesWithObstacles</t>
+  </si>
+  <si>
+    <t>Physics</t>
+  </si>
+  <si>
+    <t>Handles unique collision effects when colliding with obstacles.</t>
+  </si>
+  <si>
+    <t>TrackedInColliderContainers</t>
+  </si>
+  <si>
+    <t>Allows being tracked by ColliderContainers and tracks which ones are currently tracking it.</t>
+  </si>
+  <si>
+    <t>Collider2D</t>
+  </si>
+  <si>
+    <t>deregisterFromTrackingContainers listens to WaitInPoolEvent</t>
+  </si>
+  <si>
+    <t>ActorSpawnSettings</t>
+  </si>
+  <si>
+    <t>Spawn</t>
+  </si>
+  <si>
+    <t>SpawnEvent, Momentum, StartDelay, DelayAfterSpawn, Iteration, NumberToSpawn, Actors</t>
+  </si>
+  <si>
+    <t>ActorSpawner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spawn </t>
+  </si>
+  <si>
+    <t>Allows configuring how, when, and which actors this object spawns.</t>
+  </si>
+  <si>
+    <t>Allows an object to spawn actors when certain events occur. Contains its own static manager.</t>
+  </si>
+  <si>
+    <t>PoolToSpawnIn, ActorSpawnSettings</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,13 +331,37 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -208,10 +373,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -226,10 +393,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -542,122 +733,411 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE64B771-968C-46C8-9271-EDE5A665D12D}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.140625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="53.42578125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="51" style="7" customWidth="1"/>
-    <col min="5" max="5" width="85.28515625" style="7" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="7"/>
+    <col min="1" max="1" width="20.140625" style="10" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" style="10" customWidth="1"/>
+    <col min="3" max="3" width="47.5703125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" style="10" customWidth="1"/>
+    <col min="5" max="5" width="51" style="13" customWidth="1"/>
+    <col min="6" max="6" width="68" style="10" customWidth="1"/>
+    <col min="7" max="7" width="35.7109375" style="13" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="6" customFormat="1" ht="10.5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" s="6" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="B6" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="7" t="s">
+      <c r="D26" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>36</v>
+      <c r="E28" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A30" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G31" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G32" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G33" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G34" s="12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="F35" s="8"/>
+      <c r="G35" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More work on hardpoints, modules, spells, and UIToolkit.
</commit_message>
<xml_diff>
--- a/Stats.xlsx
+++ b/Stats.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Unity Projects\Project-SpaceMage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11F0ECC6-CC4B-48BA-873C-1CE90FC61FDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA2E1DB5-7F26-4478-9F37-2A1514F8EF56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{C7E500E0-3096-4EFE-AE2D-B6684D65CA8F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{C7E500E0-3096-4EFE-AE2D-B6684D65CA8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Functionality" sheetId="4" r:id="rId1"/>
     <sheet name="Ships" sheetId="1" r:id="rId2"/>
     <sheet name="Engines" sheetId="2" r:id="rId3"/>
-    <sheet name="Magic Spheres" sheetId="3" r:id="rId4"/>
+    <sheet name="Hardpoints" sheetId="5" r:id="rId4"/>
+    <sheet name="Magic Spheres" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="Engines">Engines!$A$2:$A$12</definedName>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="147">
   <si>
     <t>Name</t>
   </si>
@@ -296,13 +297,199 @@
   </si>
   <si>
     <t>PoolToSpawnIn, ActorSpawnSettings</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>IsExternal</t>
+  </si>
+  <si>
+    <t>Rating</t>
+  </si>
+  <si>
+    <t>Mods</t>
+  </si>
+  <si>
+    <t>Spells</t>
+  </si>
+  <si>
+    <t>Ammo</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>LightX</t>
+  </si>
+  <si>
+    <t>MedX</t>
+  </si>
+  <si>
+    <t>HeavyX</t>
+  </si>
+  <si>
+    <t>Light</t>
+  </si>
+  <si>
+    <t>Med</t>
+  </si>
+  <si>
+    <t>Heavy</t>
+  </si>
+  <si>
+    <t>l-x</t>
+  </si>
+  <si>
+    <t>m-x</t>
+  </si>
+  <si>
+    <t>h-x</t>
+  </si>
+  <si>
+    <t>* Ammo Calculation:</t>
+  </si>
+  <si>
+    <t>* Module Calculation:</t>
+  </si>
+  <si>
+    <t>Spread</t>
+  </si>
+  <si>
+    <t>RoF</t>
+  </si>
+  <si>
+    <t>* Spread Calculation:</t>
+  </si>
+  <si>
+    <t>* Rate of Fire Calculation:</t>
+  </si>
+  <si>
+    <t>* Spells Calculation:</t>
+  </si>
+  <si>
+    <t>* Spellpower Calculation:</t>
+  </si>
+  <si>
+    <t>Spellpower</t>
+  </si>
+  <si>
+    <t>i: 25%, 50%, 25%; x: 50%, 25%, 25%</t>
+  </si>
+  <si>
+    <t>l-i</t>
+  </si>
+  <si>
+    <t>m-i</t>
+  </si>
+  <si>
+    <t>h-i</t>
+  </si>
+  <si>
+    <t>i: 0; x: 0.5-1.5</t>
+  </si>
+  <si>
+    <t>ix: 0.5-1.5</t>
+  </si>
+  <si>
+    <t>ix: 25%, 50%, 25%</t>
+  </si>
+  <si>
+    <t>i: 1-2; x: 0.5-1.5</t>
+  </si>
+  <si>
+    <t>i: 0.5-1.5; x: 1-2</t>
+  </si>
+  <si>
+    <t>IsTurret</t>
+  </si>
+  <si>
+    <t>ConeRadius</t>
+  </si>
+  <si>
+    <t>LightXT</t>
+  </si>
+  <si>
+    <t>MedXT</t>
+  </si>
+  <si>
+    <t>HeavyXT</t>
+  </si>
+  <si>
+    <t>LightT</t>
+  </si>
+  <si>
+    <t>MedT</t>
+  </si>
+  <si>
+    <t>HeavyT</t>
+  </si>
+  <si>
+    <t>l-xt</t>
+  </si>
+  <si>
+    <t>m-xt</t>
+  </si>
+  <si>
+    <t>h-xt</t>
+  </si>
+  <si>
+    <t>l-it</t>
+  </si>
+  <si>
+    <t>m-it</t>
+  </si>
+  <si>
+    <t>h-it</t>
+  </si>
+  <si>
+    <t>LightXTT</t>
+  </si>
+  <si>
+    <t>MedXTT</t>
+  </si>
+  <si>
+    <t>HeavyXTT</t>
+  </si>
+  <si>
+    <t>l-xT</t>
+  </si>
+  <si>
+    <t>m-xT</t>
+  </si>
+  <si>
+    <t>h-xT</t>
+  </si>
+  <si>
+    <t>l-iT</t>
+  </si>
+  <si>
+    <t>m-iT</t>
+  </si>
+  <si>
+    <t>h-iT</t>
+  </si>
+  <si>
+    <t>LightTT</t>
+  </si>
+  <si>
+    <t>MedTT</t>
+  </si>
+  <si>
+    <t>HeavyTT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -345,8 +532,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -363,8 +565,13 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -372,13 +579,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -417,8 +640,30 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Calculation" xfId="3" builtinId="22"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -735,8 +980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE64B771-968C-46C8-9271-EDE5A665D12D}">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.25"/>
@@ -1312,6 +1557,897 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C1DFF9A-1FC7-45CB-B5D1-3338268AE014}">
+  <dimension ref="A1:L35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" s="17">
+        <v>30</v>
+      </c>
+      <c r="G2" s="17">
+        <v>1</v>
+      </c>
+      <c r="H2" s="17">
+        <v>1</v>
+      </c>
+      <c r="I2" s="17">
+        <v>1.5</v>
+      </c>
+      <c r="J2" s="17">
+        <v>2</v>
+      </c>
+      <c r="K2" s="17">
+        <v>1</v>
+      </c>
+      <c r="L2" s="17">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" s="17">
+        <v>30</v>
+      </c>
+      <c r="G3" s="17">
+        <v>1</v>
+      </c>
+      <c r="H3" s="17">
+        <v>1</v>
+      </c>
+      <c r="I3" s="17">
+        <v>1.5</v>
+      </c>
+      <c r="J3" s="17">
+        <v>2</v>
+      </c>
+      <c r="K3" s="17">
+        <v>1</v>
+      </c>
+      <c r="L3" s="17">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" s="17">
+        <v>30</v>
+      </c>
+      <c r="G4" s="17">
+        <v>1</v>
+      </c>
+      <c r="H4" s="17">
+        <v>1</v>
+      </c>
+      <c r="I4" s="17">
+        <v>1.5</v>
+      </c>
+      <c r="J4" s="17">
+        <v>2</v>
+      </c>
+      <c r="K4" s="17">
+        <v>1</v>
+      </c>
+      <c r="L4" s="17">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" s="17">
+        <v>180</v>
+      </c>
+      <c r="G5" s="17">
+        <v>0</v>
+      </c>
+      <c r="H5" s="17">
+        <v>1</v>
+      </c>
+      <c r="I5" s="17">
+        <v>1</v>
+      </c>
+      <c r="J5" s="17">
+        <v>1</v>
+      </c>
+      <c r="K5" s="17">
+        <v>1</v>
+      </c>
+      <c r="L5" s="17">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" s="17">
+        <v>180</v>
+      </c>
+      <c r="G6" s="17">
+        <v>0</v>
+      </c>
+      <c r="H6" s="17">
+        <v>1</v>
+      </c>
+      <c r="I6" s="17">
+        <v>1</v>
+      </c>
+      <c r="J6" s="17">
+        <v>1</v>
+      </c>
+      <c r="K6" s="17">
+        <v>1</v>
+      </c>
+      <c r="L6" s="17">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" s="17">
+        <v>180</v>
+      </c>
+      <c r="G7" s="17">
+        <v>0</v>
+      </c>
+      <c r="H7" s="17">
+        <v>1</v>
+      </c>
+      <c r="I7" s="17">
+        <v>1</v>
+      </c>
+      <c r="J7" s="17">
+        <v>1</v>
+      </c>
+      <c r="K7" s="17">
+        <v>1</v>
+      </c>
+      <c r="L7" s="17">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" s="17">
+        <v>360</v>
+      </c>
+      <c r="G8" s="17">
+        <v>0</v>
+      </c>
+      <c r="H8" s="17">
+        <v>1</v>
+      </c>
+      <c r="I8" s="17">
+        <v>1</v>
+      </c>
+      <c r="J8" s="17">
+        <v>0</v>
+      </c>
+      <c r="K8" s="17">
+        <v>1</v>
+      </c>
+      <c r="L8" s="17">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="D9" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9" s="17">
+        <v>360</v>
+      </c>
+      <c r="G9" s="17">
+        <v>0</v>
+      </c>
+      <c r="H9" s="17">
+        <v>1</v>
+      </c>
+      <c r="I9" s="17">
+        <v>1</v>
+      </c>
+      <c r="J9" s="17">
+        <v>0</v>
+      </c>
+      <c r="K9" s="17">
+        <v>1</v>
+      </c>
+      <c r="L9" s="17">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="D10" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F10" s="17">
+        <v>360</v>
+      </c>
+      <c r="G10" s="17">
+        <v>0</v>
+      </c>
+      <c r="H10" s="17">
+        <v>1</v>
+      </c>
+      <c r="I10" s="17">
+        <v>1</v>
+      </c>
+      <c r="J10" s="17">
+        <v>0</v>
+      </c>
+      <c r="K10" s="17">
+        <v>1</v>
+      </c>
+      <c r="L10" s="17">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="D11" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="F11" s="17">
+        <v>30</v>
+      </c>
+      <c r="G11" s="17">
+        <v>2</v>
+      </c>
+      <c r="H11" s="17">
+        <v>1</v>
+      </c>
+      <c r="I11" s="17">
+        <v>1.5</v>
+      </c>
+      <c r="J11" s="17">
+        <v>2</v>
+      </c>
+      <c r="K11" s="17">
+        <v>1.5</v>
+      </c>
+      <c r="L11" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="D12" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="F12" s="17">
+        <v>30</v>
+      </c>
+      <c r="G12" s="17">
+        <v>2</v>
+      </c>
+      <c r="H12" s="17">
+        <v>1</v>
+      </c>
+      <c r="I12" s="17">
+        <v>1.5</v>
+      </c>
+      <c r="J12" s="17">
+        <v>2</v>
+      </c>
+      <c r="K12" s="17">
+        <v>1.5</v>
+      </c>
+      <c r="L12" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="D13" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="F13" s="17">
+        <v>30</v>
+      </c>
+      <c r="G13" s="17">
+        <v>2</v>
+      </c>
+      <c r="H13" s="17">
+        <v>1</v>
+      </c>
+      <c r="I13" s="17">
+        <v>1.5</v>
+      </c>
+      <c r="J13" s="17">
+        <v>2</v>
+      </c>
+      <c r="K13" s="17">
+        <v>1.5</v>
+      </c>
+      <c r="L13" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="D14" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E14" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F14" s="17">
+        <v>180</v>
+      </c>
+      <c r="G14" s="17">
+        <v>1</v>
+      </c>
+      <c r="H14" s="17">
+        <v>1</v>
+      </c>
+      <c r="I14" s="17">
+        <v>1</v>
+      </c>
+      <c r="J14" s="17">
+        <v>1</v>
+      </c>
+      <c r="K14" s="17">
+        <v>1.5</v>
+      </c>
+      <c r="L14" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="D15" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E15" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F15" s="17">
+        <v>180</v>
+      </c>
+      <c r="G15" s="17">
+        <v>1</v>
+      </c>
+      <c r="H15" s="17">
+        <v>1</v>
+      </c>
+      <c r="I15" s="17">
+        <v>1</v>
+      </c>
+      <c r="J15" s="17">
+        <v>1</v>
+      </c>
+      <c r="K15" s="17">
+        <v>1.5</v>
+      </c>
+      <c r="L15" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="D16" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E16" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F16" s="17">
+        <v>180</v>
+      </c>
+      <c r="G16" s="17">
+        <v>1</v>
+      </c>
+      <c r="H16" s="17">
+        <v>1</v>
+      </c>
+      <c r="I16" s="17">
+        <v>1</v>
+      </c>
+      <c r="J16" s="17">
+        <v>1</v>
+      </c>
+      <c r="K16" s="17">
+        <v>1.5</v>
+      </c>
+      <c r="L16" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="D17" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E17" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F17" s="17">
+        <v>360</v>
+      </c>
+      <c r="G17" s="17">
+        <v>1</v>
+      </c>
+      <c r="H17" s="17">
+        <v>1</v>
+      </c>
+      <c r="I17" s="17">
+        <v>1</v>
+      </c>
+      <c r="J17" s="17">
+        <v>0</v>
+      </c>
+      <c r="K17" s="17">
+        <v>1.5</v>
+      </c>
+      <c r="L17" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="D18" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E18" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F18" s="17">
+        <v>360</v>
+      </c>
+      <c r="G18" s="17">
+        <v>1</v>
+      </c>
+      <c r="H18" s="17">
+        <v>1</v>
+      </c>
+      <c r="I18" s="17">
+        <v>1</v>
+      </c>
+      <c r="J18" s="17">
+        <v>0</v>
+      </c>
+      <c r="K18" s="17">
+        <v>1.5</v>
+      </c>
+      <c r="L18" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="D19" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E19" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F19" s="17">
+        <v>360</v>
+      </c>
+      <c r="G19" s="17">
+        <v>1</v>
+      </c>
+      <c r="H19" s="17">
+        <v>1</v>
+      </c>
+      <c r="I19" s="17">
+        <v>1</v>
+      </c>
+      <c r="J19" s="17">
+        <v>0</v>
+      </c>
+      <c r="K19" s="17">
+        <v>1.5</v>
+      </c>
+      <c r="L19" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="19"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="18"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="19"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="18"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="19"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="18"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="19"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="19"/>
+      <c r="L23" s="18"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="19"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="19"/>
+      <c r="L24" s="18"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="19"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="18"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="20"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="19"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="18"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="18"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="19"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="19"/>
+      <c r="L28" s="18"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="E30" s="18"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="E31" s="18"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="E32" s="18"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="B33" s="20"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="E33" s="18"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="E34" s="18"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="B35" s="20"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="E35" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A33:C33"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F9F5913-872F-4EF1-9FC5-09C660CB0FB2}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>